<commit_message>
Readme updates - Quantitative evaluation - Contents page - Instructions - Other small edits to requirements and implementation sections
</commit_message>
<xml_diff>
--- a/Evaluation/NASA TLX analysis.xlsx
+++ b/Evaluation/NASA TLX analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liz\Documents\ComputerScienceMSc\Overview of Software Engineering\Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liz\Documents\ComputerScienceMSc\Overview of Software Engineering\2024-group-9\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20282139-DD2C-4375-B2AE-4C53182B4FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C12A1D5-6359-44FF-B859-64D9112178A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F55ED75C-09FF-4582-8DDC-A085A746E3FA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
   <si>
     <t>Easy</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>To past into calculator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average score </t>
   </si>
 </sst>
 </file>
@@ -123,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,9 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0722FD3-59B4-44EB-9224-A1A2030B8837}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -563,11 +565,11 @@
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R9" si="2">SUMIF($A$4:$A$39,$Q5,F$4:F$39)</f>
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S9" si="3">SUMIF($A$4:$A$39,$Q5,G$4:G$39)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -635,11 +637,11 @@
       </c>
       <c r="R7">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="S7">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -768,11 +770,11 @@
       </c>
       <c r="R11" t="str">
         <f>R4&amp;", "&amp;R5&amp;", "&amp;R6&amp;", "&amp;R7&amp;", "&amp;R8&amp;", "&amp;R9</f>
-        <v>235, 260, 230, 230, 330, 115</v>
+        <v>235, 255, 230, 200, 330, 115</v>
       </c>
       <c r="S11" t="str">
         <f>S4&amp;", "&amp;S5&amp;", "&amp;S6&amp;", "&amp;S7&amp;", "&amp;S8&amp;", "&amp;S9</f>
-        <v>495, 255, 220, 195, 430, 210</v>
+        <v>495, 260, 220, 225, 430, 210</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -861,18 +863,21 @@
         <v>8</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>40</v>
+      <c r="R15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -899,8 +904,17 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -924,8 +938,19 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>4</v>
+      </c>
+      <c r="R17" s="1">
+        <f>SUMIF($C$4:$C$39,$Q17,F$4:F$39)/6</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="S17" s="1">
+        <f>SUMIF($C$4:$C$39,$Q17,G$4:G$39)/6</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -949,8 +974,19 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>3</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" ref="R18:S22" si="4">SUMIF($C$4:$C$39,$Q18,F$4:F$39)/6</f>
+        <v>30.833333333333332</v>
+      </c>
+      <c r="S18" s="1">
+        <f t="shared" si="4"/>
+        <v>40.833333333333336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -974,8 +1010,19 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="4"/>
+        <v>29.166666666666668</v>
+      </c>
+      <c r="S19" s="1">
+        <f t="shared" si="4"/>
+        <v>41.666666666666664</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -999,8 +1046,19 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>6</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="4"/>
+        <v>35.833333333333336</v>
+      </c>
+      <c r="S20" s="1">
+        <f t="shared" si="4"/>
+        <v>54.166666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1024,8 +1082,19 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="S21" s="1">
+        <f t="shared" si="4"/>
+        <v>59.166666666666664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1049,8 +1118,19 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>8</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="S22" s="1">
+        <f t="shared" si="4"/>
+        <v>48.333333333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1075,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1100,7 +1180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1111,21 +1191,21 @@
         <v>6</v>
       </c>
       <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
         <v>16</v>
       </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
       <c r="F25">
         <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="G25">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1150,7 +1230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1175,7 +1255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
@@ -1200,7 +1280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1225,7 +1305,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1250,7 +1330,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1275,7 +1355,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1477,5 +1557,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>